<commit_message>
added login, register and other common pages
</commit_message>
<xml_diff>
--- a/ResumeProcessing/Extracted Data/Extracted.xlsx
+++ b/ResumeProcessing/Extracted Data/Extracted.xlsx
@@ -7,10 +7,11 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-09-01" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-08-31" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-08-29" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-04" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-09-01" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-08-31" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-08-29" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -416,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,58 +455,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Html, Programming, Website, Engineering, Python, Technical, Database, Editing, Video, Training, English, Php, Analysis, Networking, Writing, C, Tensorflow, Content, Research, Css</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>athale20comp@student.mes.ac.in</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Design, Html, Css, System, Php, Java, Programming, Engineering, Python, Flask, Django, Javascript, C</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>pranjupolawar27@gmail.com</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>7058168004</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Github, Design, English, Html, Css, Website, Programming, Engineering, Python, Technical, Algorithms, Sql, Testing, C</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>maheshwariudhayan1@gmail.com</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>9975635803</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>International, Github, Content, English, Design, Html, Css, Website, Programming, Engineering, Python, Technical, Algorithms, Networking, Editing, Testing, Photography, C</t>
+          <t>Editing, Programming, English, Python, Css, Content, Training, Networking, Research, Database, Engineering, Php, Website, Analysis, Tensorflow, C, Html, Technical, Writing, Video</t>
         </is>
       </c>
     </row>
@@ -520,7 +470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,34 +498,68 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>athale20comp@student.mes.ac.in</t>
+          <t>maheshkulkarni01121@gmail.com</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+918605131403</t>
+          <t>9423627124</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Python, Java, System, Php, Design, C, Programming, Javascript, Html, Flask, Django, Engineering, Css</t>
+          <t>Html, Programming, Website, Engineering, Python, Technical, Database, Editing, Video, Training, English, Php, Analysis, Networking, Writing, C, Tensorflow, Content, Research, Css</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>maheshkulkarni01121@gmail.com</t>
+          <t>athale20comp@student.mes.ac.in</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>9423627124</t>
+          <t>+918605131403</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Technical, Html, Website, Css, English, Python, Analysis, C, Tensorflow, Programming, Video, Editing, Research, Networking, Training, Php, Content, Writing, Database, Engineering</t>
+          <t>Design, Html, Css, System, Php, Java, Programming, Engineering, Python, Flask, Django, Javascript, C</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>pranjupolawar27@gmail.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>7058168004</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Github, Design, English, Html, Css, Website, Programming, Engineering, Python, Technical, Algorithms, Sql, Testing, C</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>maheshwariudhayan1@gmail.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9975635803</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>International, Github, Content, English, Design, Html, Css, Website, Programming, Engineering, Python, Technical, Algorithms, Networking, Editing, Testing, Photography, C</t>
         </is>
       </c>
     </row>
@@ -628,7 +612,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Java, Django, C, Php, System, Engineering, Design, Html, Flask, Javascript, Python, Css, Programming</t>
+          <t>Python, Java, System, Php, Design, C, Programming, Javascript, Html, Flask, Django, Engineering, Css</t>
         </is>
       </c>
     </row>
@@ -645,7 +629,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Tensorflow, Analysis, Video, C, Php, Database, Engineering, Training, Website, Writing, Technical, English, Research, Programming, Editing, Content, Html, Css, Networking, Python</t>
+          <t>Technical, Html, Website, Css, English, Python, Analysis, C, Tensorflow, Programming, Video, Editing, Research, Networking, Training, Php, Content, Writing, Database, Engineering</t>
         </is>
       </c>
     </row>
@@ -655,6 +639,76 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>athale20comp@student.mes.ac.in</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Java, Django, C, Php, System, Engineering, Design, Html, Flask, Javascript, Python, Css, Programming</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Tensorflow, Analysis, Video, C, Php, Database, Engineering, Training, Website, Writing, Technical, English, Research, Programming, Editing, Content, Html, Css, Networking, Python</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
resolved the json error and made a copy of current parser notebook into outermost folder
</commit_message>
<xml_diff>
--- a/ResumeProcessing/Extracted Data/Extracted.xlsx
+++ b/ResumeProcessing/Extracted Data/Extracted.xlsx
@@ -7,11 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-04" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-09-01" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-08-31" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-08-29" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-16" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-04" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-09-01" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-08-31" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-08-29" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -443,19 +444,9 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>9423627124</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Editing, Programming, English, Python, Css, Content, Training, Networking, Research, Database, Engineering, Php, Website, Analysis, Tensorflow, C, Html, Technical, Writing, Video</t>
+          <t>R, C, P</t>
         </is>
       </c>
     </row>
@@ -465,6 +456,59 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Editing, Programming, English, Python, Css, Content, Training, Networking, Research, Database, Engineering, Php, Website, Analysis, Tensorflow, C, Html, Technical, Writing, Video</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -560,76 +604,6 @@
       <c r="C5" t="inlineStr">
         <is>
           <t>International, Github, Content, English, Design, Html, Css, Website, Programming, Engineering, Python, Technical, Algorithms, Networking, Editing, Testing, Photography, C</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Mobile No.</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Skills</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>athale20comp@student.mes.ac.in</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Python, Java, System, Php, Design, C, Programming, Javascript, Html, Flask, Django, Engineering, Css</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>9423627124</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Technical, Html, Website, Css, English, Python, Analysis, C, Tensorflow, Programming, Video, Editing, Research, Networking, Training, Php, Content, Writing, Database, Engineering</t>
         </is>
       </c>
     </row>
@@ -682,7 +656,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Java, Django, C, Php, System, Engineering, Design, Html, Flask, Javascript, Python, Css, Programming</t>
+          <t>Python, Java, System, Php, Design, C, Programming, Javascript, Html, Flask, Django, Engineering, Css</t>
         </is>
       </c>
     </row>
@@ -699,7 +673,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Tensorflow, Analysis, Video, C, Php, Database, Engineering, Training, Website, Writing, Technical, English, Research, Programming, Editing, Content, Html, Css, Networking, Python</t>
+          <t>Technical, Html, Website, Css, English, Python, Analysis, C, Tensorflow, Programming, Video, Editing, Research, Networking, Training, Php, Content, Writing, Database, Engineering</t>
         </is>
       </c>
     </row>
@@ -709,6 +683,76 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>athale20comp@student.mes.ac.in</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Java, Django, C, Php, System, Engineering, Design, Html, Flask, Javascript, Python, Css, Programming</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Tensorflow, Analysis, Video, C, Php, Database, Engineering, Training, Website, Writing, Technical, English, Research, Programming, Editing, Content, Html, Css, Networking, Python</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
madhe python file for parser
</commit_message>
<xml_diff>
--- a/ResumeProcessing/Extracted Data/Extracted.xlsx
+++ b/ResumeProcessing/Extracted Data/Extracted.xlsx
@@ -1,18 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-16" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-04" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-09-01" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-08-31" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-08-29" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="2023-10-22" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2023-10-21" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2023-10-19" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="2023-10-16" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="2023-10-04" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="2023-09-01" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="2023-08-31" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="2023-08-29" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Sheet" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -418,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,9 +447,104 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>R, C, P</t>
+          <t>Website, Editing, Research, Engineering, Python, Programming, Tensorflow, Networking, Training, Html, C, Writing, Database, Analysis, Video, Content, Css, English, Php, Technical</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Php, Video, English, Css, Html, Technical, Website, Editing, Analysis, Tensorflow, Networking, Python, Programming, Research, C, Engineering, Training, Writing, Content, Database</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Networking, Editing, Website, Programming, C, Html, Css, Database, Technical, Tensorflow, Analysis, English, Php, Research, Python, Engineering, Writing, Video, Training, Content</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Html, Database, Writing, Editing, Website, Technical, Content, English, Engineering, Css, C, Video, Training, Python, Php, Analysis, Programming, Tensorflow, Networking, Research</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Technical, Php, Tensorflow, English, Programming, Engineering, C, Networking, Training, Website, Html, Python, Editing, Video, Analysis, Database, Research, Css, Content, Writing</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Website, Content, Networking, Programming, Css, C, Training, Python, Writing, Research, Html, Engineering, Analysis, Editing, Video, Php, English, Technical, Tensorflow, Database</t>
         </is>
       </c>
     </row>
@@ -456,6 +554,178 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>R, C, P</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>P, C, R</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Html, Css, Website, English, Analysis, Training, Engineering, C, Editing, Php, Writing, Database, Video, Networking, Tensorflow, Research, Programming, Technical, Python, Content</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Research, Html, Css, Php, Tensorflow, Networking, Database, Content, Website, Analysis, Python, C, Engineering, Training, Technical, English, Writing, Editing, Programming, Video</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Writing, C, Css, Research, Editing, Php, Training, Database, Technical, English, Analysis, Tensorflow, Video, Html, Content, Website, Programming, Python, Engineering, Networking</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>C, P, R</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>C, R, P</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>C, R, P</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>C, R, P</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>C, R, P</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -487,19 +757,9 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>9423627124</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Editing, Programming, English, Python, Css, Content, Training, Networking, Research, Database, Engineering, Php, Website, Analysis, Tensorflow, C, Html, Technical, Writing, Video</t>
+          <t>R, C, P</t>
         </is>
       </c>
     </row>
@@ -508,7 +768,60 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Editing, Programming, English, Python, Css, Content, Training, Networking, Research, Database, Engineering, Php, Website, Analysis, Tensorflow, C, Html, Technical, Writing, Video</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -612,7 +925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -682,7 +995,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -752,7 +1065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
name and matched percentage in excel sheet and half code for display matched percent
</commit_message>
<xml_diff>
--- a/ResumeProcessing/Extracted Data/Extracted.xlsx
+++ b/ResumeProcessing/Extracted Data/Extracted.xlsx
@@ -7,15 +7,17 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="2023-10-22" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="2023-10-21" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="2023-10-19" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="2023-10-16" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="2023-10-04" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="2023-09-01" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="2023-08-31" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="2023-08-29" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Sheet" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="2023-11-041" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2023-11-04" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2023-10-22" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="2023-10-21" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="2023-10-19" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="2023-10-16" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="2023-10-04" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="2023-09-01" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="2023-08-31" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="2023-08-29" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Sheet" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -421,6 +423,422 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email Id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Matched</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Networking, Tensorflow, Queries, Content, Sql, Pandas, Technical, Php, Python, Html, Mining, Training, Logbook, Jupyter, Css, Numpy, C, Analytics, Mysql, Database, Certification, Nltk, Reports, Process, Engineering, Spacy, Analysis, Matplotlib, Javascript, Warehouse, Website, Research, C++, Design, Programming</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>66.66666666666666</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>athale20comp@student.mes.ac.in</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Java, Django, C, Php, System, Engineering, Design, Html, Flask, Javascript, Python, Css, Programming</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Tensorflow, Analysis, Video, C, Php, Database, Engineering, Training, Website, Writing, Technical, English, Research, Programming, Editing, Content, Html, Css, Networking, Python</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Analysis, Training, C, Writing, Html, Engineering, Tensorflow, Programming, Website, Video, English, Php, Python, Networking, Content, Editing, Database, Research, Technical, Css</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Sakshi Patil</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Pandas, Python, Training, Design, Php, Networking, Technical, Queries, Certification, Process, C++, Numpy, Javascript, Mining, Sql, Analysis, Matplotlib, Reports, Logbook, Spacy, Tensorflow, Research, Warehouse, Nltk, C, Engineering, Mysql, Html, Programming, Content, Database, Jupyter, Css, Analytics, Website</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Sakshi Patil</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Process, Sql, Content, Warehouse, Matplotlib, Javascript, C++, Website, Design, Training, Analysis, Networking, Programming, Python, Mysql, Mining, Technical, Css, Logbook, Numpy, Jupyter, Analytics, C, Reports, Certification, Nltk, Pandas, Spacy, Engineering, Html, Database, Tensorflow, Php, Queries, Research</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Javascript, Php, Certification, Technical, Research, Html, Analysis, Queries, Tensorflow, Networking, C++, Mysql, Content, Jupyter, Pandas, Python, Mining, Numpy, Analytics, Programming, Spacy, Database, Logbook, Process, Design, Matplotlib, Website, Engineering, C, Sql, Reports, Warehouse, Training, Css, Nltk</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>66.66666666666666</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Website, Analysis, Training, Database, Certification, Reports, C, Networking, Engineering, Javascript, Php, Analytics, Jupyter, C++, Process, Pandas, Tensorflow, Logbook, Programming, Html, Queries, Spacy, Warehouse, Content, Mysql, Nltk, Numpy, Research, Mining, Sql, Css, Python, Design, Technical, Matplotlib</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>66.66666666666666</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Pandas, Spacy, Logbook, Certification, Matplotlib, C, Training, Networking, Website, Sql, Html, C++, Reports, Programming, Tensorflow, Mining, Warehouse, Nltk, Javascript, Numpy, Css, Mysql, Design, Analysis, Jupyter, Php, Technical, Research, Queries, Python, Database, Engineering, Content, Process, Analytics</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>66.66666666666666</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Database, Python, Process, Training, Sql, Css, Matplotlib, Numpy, Engineering, Research, Programming, Technical, Pandas, Certification, Networking, C++, Queries, Javascript, Analytics, C, Warehouse, Logbook, Reports, Nltk, Php, Analysis, Tensorflow, Html, Design, Spacy, Jupyter, Mining, Website, Content, Mysql</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>66.66666666666666</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Mysql, Training, Logbook, Content, Mining, Analytics, Process, Certification, Website, Jupyter, Warehouse, Javascript, Analysis, Queries, Reports, Html, Networking, Programming, Engineering, Design, Css, Tensorflow, Technical, Pandas, Database, Matplotlib, C++, Research, Nltk, Sql, Php, Python, Numpy, Spacy, C</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>66.66666666666666</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Analytics, Css, Tensorflow, Sql, Database, Python, Programming, Matplotlib, Engineering, C, Process, Networking, Jupyter, Html, Queries, Website, Research, Certification, Technical, Reports, Design, Numpy, Warehouse, Logbook, Spacy, Javascript, Analysis, Nltk, Training, Mysql, Pandas, Mining, Php, C++, Content</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>66.66666666666666</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -553,7 +971,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -654,7 +1072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -725,7 +1143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -768,7 +1186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -821,7 +1239,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -925,7 +1343,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -993,92 +1411,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Mobile No.</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Skills</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>athale20comp@student.mes.ac.in</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Java, Django, C, Php, System, Engineering, Design, Html, Flask, Javascript, Python, Css, Programming</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>9423627124</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Tensorflow, Analysis, Video, C, Php, Database, Engineering, Training, Website, Writing, Technical, English, Research, Programming, Editing, Content, Html, Css, Networking, Python</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>